<commit_message>
ci: update TAS forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Cote d'Ivoire/Apr 2024/ci_lf_tas1_202404_2_partcipants.xlsx
+++ b/LF/TAS/Cote d'Ivoire/Apr 2024/ci_lf_tas1_202404_2_partcipants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Cote d'Ivoire\Apr 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AC55E7-0485-423B-B95B-4251D1D2FAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395E251D-3647-4C1C-A0A3-F2E455A27678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="84">
   <si>
     <t>type</t>
   </si>
@@ -117,18 +117,6 @@
     <t>Sélectionner le code de votre école</t>
   </si>
   <si>
-    <t>${p_cluster_name} != 'Autre'</t>
-  </si>
-  <si>
-    <t>p_cluster_name2</t>
-  </si>
-  <si>
-    <t>${p_cluster_name} = 'Autre'</t>
-  </si>
-  <si>
-    <t>p_cluster_id2</t>
-  </si>
-  <si>
     <t>select_one yes_no</t>
   </si>
   <si>
@@ -195,9 +183,6 @@
     <t>Code d'identification du répondant (Veuillez recopier ce code tel qu'il est quelque part entre autre sur les test de diagnostique)</t>
   </si>
   <si>
-    <t>if(${p_cluster_name} = 'Autre', concat(${p_district_id}, '-', ${p_cluster_id2}, '-' ,${p_num}), concat(${p_district_id}, '-', ${p_cluster_id}, '-' ,${p_num}))</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
@@ -282,10 +267,13 @@
     <t>French</t>
   </si>
   <si>
-    <t>ci_lf_tas1_202404_2_partcipants</t>
-  </si>
-  <si>
-    <t>(2024 Avr) 2. TAS1 FL - Participants</t>
+    <t xml:space="preserve"> concat(${p_district_id}, '-', ${p_cluster_id}, '-' ,${p_num})</t>
+  </si>
+  <si>
+    <t>(2024 Avr) 2. TAS1 &amp; 2 FL - Participants V2</t>
+  </si>
+  <si>
+    <t>ci_lf_tas1_202404_2_partcipants_v2</t>
   </si>
 </sst>
 </file>
@@ -398,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -426,9 +414,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -732,13 +717,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" activeCellId="1" sqref="C1:D1048576 I1:I1048576"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -765,10 +750,10 @@
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
@@ -806,17 +791,17 @@
       <c r="B2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="10"/>
@@ -835,13 +820,13 @@
       <c r="B3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="18"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="10"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="21"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="20"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
       <c r="J3" s="11" t="s">
@@ -858,13 +843,13 @@
       <c r="B4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="18"/>
+      <c r="D4" s="17"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="21"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="11" t="s">
@@ -881,13 +866,13 @@
       <c r="B5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="17"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="11" t="s">
@@ -904,13 +889,13 @@
       <c r="B6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="18"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="21"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="11" t="s">
@@ -932,9 +917,7 @@
       </c>
       <c r="D7" s="12"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="H7" s="8"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12" t="s">
         <v>19</v>
@@ -942,55 +925,75 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:13" s="8" customFormat="1">
-      <c r="A8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="13" t="s">
+    <row r="8" spans="1:13" s="3" customFormat="1">
+      <c r="A8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="8" t="s">
+      <c r="C8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="D8" s="17"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" s="8" customFormat="1">
-      <c r="A9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="14" t="s">
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="1:13" s="3" customFormat="1">
+      <c r="A9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="8" t="s">
+      <c r="B9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" s="3" customFormat="1">
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="1:13" s="3" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11" t="s">
         <v>19</v>
@@ -999,230 +1002,176 @@
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:13" s="3" customFormat="1">
+    <row r="11" spans="1:13" s="3" customFormat="1" ht="31.5">
       <c r="A11" s="10" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="11"/>
+        <v>42</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="10"/>
       <c r="J11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A12" s="10" t="s">
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="1:13" s="3" customFormat="1" ht="31.5">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11" t="s">
+      <c r="B12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-    </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" ht="31.5">
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+    </row>
+    <row r="13" spans="1:13" s="3" customFormat="1" ht="47.25">
       <c r="A13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="17"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>81</v>
+      </c>
       <c r="J13" s="11" t="s">
         <v>19</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
+      <c r="M13" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" ht="31.5">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="3" t="s">
+      <c r="A14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-    </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" ht="63">
+      <c r="C14" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+    </row>
+    <row r="15" spans="1:13" s="3" customFormat="1">
       <c r="A15" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="18"/>
+        <v>57</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="17"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>19</v>
-      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
-      <c r="M15" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" ht="31.5">
+      <c r="M15" s="10"/>
+    </row>
+    <row r="16" spans="1:13" s="3" customFormat="1">
       <c r="A16" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="18"/>
+        <v>61</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="H16" s="10"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="11"/>
+      <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" s="3" customFormat="1">
+    <row r="17" spans="1:13">
       <c r="A17" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-    </row>
-    <row r="18" spans="1:13" s="3" customFormat="1">
-      <c r="A18" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1234,7 +1183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
@@ -1248,7 +1197,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -1260,68 +1209,68 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1336,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1349,24 +1298,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>